<commit_message>
fluorescentie waardes verberterd, losse functie voor geschreven. Nu readme file aangepast zodat ik dat later kan nabootsen. Drugscreen files aangepast zodat je niet meer steeds de max_conc heoft te definieren
</commit_message>
<xml_diff>
--- a/resources/standard_file.xlsx
+++ b/resources/standard_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BC1B3-B9CF-EA4F-9E19-819D14FC1039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05872AB9-6D6F-9F45-9455-FDE91FCCA3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34020" yWindow="-2720" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Organoid</t>
   </si>
@@ -99,7 +99,10 @@
     <t>DX</t>
   </si>
   <si>
-    <t>Null</t>
+    <t>condition_string</t>
+  </si>
+  <si>
+    <t>conc_condition</t>
   </si>
 </sst>
 </file>
@@ -433,15 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,49 +473,52 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -580,6 +586,9 @@
         <v>0.01</v>
       </c>
       <c r="W2">
+        <v>0.01</v>
+      </c>
+      <c r="X2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update scripts and folder structure, exclude data and html files
</commit_message>
<xml_diff>
--- a/resources/standard_file.xlsx
+++ b/resources/standard_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED45551-5D81-4B47-AE9B-8E0160A1EFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A32138-D0CE-724D-ACB4-E79F59542276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34020" yWindow="500" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,18 @@
     <t>Timepoint</t>
   </si>
   <si>
+    <t>Dispensed
+well</t>
+  </si>
+  <si>
+    <t>Dispensed
+row</t>
+  </si>
+  <si>
+    <t>Dispensed
+col</t>
+  </si>
+  <si>
     <t>Value</t>
   </si>
   <si>
@@ -43,9 +55,15 @@
     <t>Concentration</t>
   </si>
   <si>
+    <t>conc_5-FU</t>
+  </si>
+  <si>
     <t>conc_Oxaliplatin</t>
   </si>
   <si>
+    <t>conc_SN-38</t>
+  </si>
+  <si>
     <t>conc_Lapatinib</t>
   </si>
   <si>
@@ -76,30 +94,13 @@
     <t>conc_condition</t>
   </si>
   <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <t>Tween</t>
+  </si>
+  <si>
     <t>DMSO_pct</t>
-  </si>
-  <si>
-    <t>Dispensed_well</t>
-  </si>
-  <si>
-    <t>Dispensed_row</t>
-  </si>
-  <si>
-    <t>Dispensed_col</t>
-  </si>
-  <si>
-    <t>conc_5FU</t>
-  </si>
-  <si>
-    <t>conc_SN38</t>
-  </si>
-  <si>
-    <t>Volume (nL)
-DMSO normalization</t>
-  </si>
-  <si>
-    <t>Volume (nL)
-a+Tw normalization</t>
   </si>
 </sst>
 </file>
@@ -436,15 +437,10 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -454,70 +450,70 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -525,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -546,7 +542,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J2">
         <v>0.01</v>

</xml_diff>